<commit_message>
Add investment case study
</commit_message>
<xml_diff>
--- a/data/rings_base_example/Global_Parameters.xlsx
+++ b/data/rings_base_example/Global_Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon Malacek\Code\LEGO-Pyomo\data\rings_base_example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{435EB99E-0A93-4518-9877-9E3C282F124E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16865058-F36D-44F0-927E-E6232DF3FC56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="0" windowWidth="38385" windowHeight="22545" tabRatio="851" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="110" yWindow="2390" windowWidth="28800" windowHeight="15380" tabRatio="851" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global Parameters" sheetId="121" r:id="rId1"/>
@@ -802,28 +802,28 @@
   <dimension ref="B1:H19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.8984375" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.59765625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.296875" style="1" customWidth="1"/>
     <col min="3" max="3" width="31" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.09765625" style="1" customWidth="1"/>
     <col min="5" max="5" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="120.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.85546875" style="1"/>
+    <col min="6" max="6" width="120.8984375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.8984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:8" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
         <v>10</v>
       </c>
@@ -843,7 +843,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>21</v>
       </c>
@@ -855,7 +855,7 @@
       <c r="G4" s="11"/>
       <c r="H4" s="14"/>
     </row>
-    <row r="5" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>23</v>
       </c>
@@ -875,12 +875,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="H6" s="13"/>
     </row>
-    <row r="7" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
@@ -891,7 +891,7 @@
       <c r="F7" s="11"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
@@ -911,12 +911,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="7" t="s">
         <v>28</v>
       </c>
@@ -926,7 +926,7 @@
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
     </row>
-    <row r="11" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
         <v>29</v>
       </c>
@@ -938,12 +938,12 @@
       <c r="G11" s="11"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C12" s="9">
-        <v>1E-3</v>
+        <v>1</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>32</v>
@@ -958,12 +958,12 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
         <v>34</v>
       </c>
@@ -974,12 +974,12 @@
       <c r="F14" s="11"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C15" s="9">
-        <v>9.9999999999999995E-7</v>
+        <v>1</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>37</v>
@@ -994,7 +994,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="17" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="7" t="s">
         <v>5</v>
       </c>
@@ -1002,7 +1002,7 @@
       <c r="F17" s="12"/>
       <c r="H17" s="16"/>
     </row>
-    <row r="18" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="5" t="s">
         <v>14</v>
       </c>
@@ -1013,7 +1013,7 @@
       <c r="F18" s="11"/>
       <c r="H18" s="13"/>
     </row>
-    <row r="19" spans="2:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:8" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
         <v>15</v>
       </c>

</xml_diff>